<commit_message>
adjusted indexing for time lagged variables
</commit_message>
<xml_diff>
--- a/GeneticProgrammingPortfolio/experiment-data/2 - stats/90/16-55-29 - with avg, min, and max/data-full.xlsx
+++ b/GeneticProgrammingPortfolio/experiment-data/2 - stats/90/16-55-29 - with avg, min, and max/data-full.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20265" windowHeight="8055" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20265" windowHeight="8055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Best Ind Training" sheetId="2" r:id="rId1"/>
     <sheet name="Ensemble in Training" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Data" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -207,7 +207,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$1</c:f>
+              <c:f>Data!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -230,7 +230,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$775</c:f>
+              <c:f>Data!$A$2:$A$775</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="774"/>
@@ -2571,7 +2571,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Data!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2594,7 +2594,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$775</c:f>
+              <c:f>Data!$B$2:$B$775</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="774"/>
@@ -4686,7 +4686,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Data!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4709,7 +4709,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$775</c:f>
+              <c:f>Data!$C$2:$C$775</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="774"/>
@@ -5214,7 +5214,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$698:$A$775</c:f>
+              <c:f>Data!$A$698:$A$775</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="78"/>
@@ -5479,7 +5479,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$698:$D$775</c:f>
+              <c:f>Data!$D$698:$D$775</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="78"/>
@@ -5744,7 +5744,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$698:$E$775</c:f>
+              <c:f>Data!$E$698:$E$775</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="78"/>
@@ -6009,7 +6009,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$698:$F$775</c:f>
+              <c:f>Data!$F$698:$F$775</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="78"/>
@@ -6274,7 +6274,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$698:$G$775</c:f>
+              <c:f>Data!$G$698:$G$775</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="78"/>
@@ -7841,7 +7841,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8201,8 +8201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K775"/>
   <sheetViews>
-    <sheetView topLeftCell="A739" workbookViewId="0">
-      <selection activeCell="D698" activeCellId="1" sqref="A698:A775 D698:G775"/>
+    <sheetView tabSelected="1" topLeftCell="A670" workbookViewId="0">
+      <selection activeCell="J698" sqref="J698"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>